<commit_message>
Updates to WEX sim card filtering
</commit_message>
<xml_diff>
--- a/input/eod/data.xlsx
+++ b/input/eod/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.franco\Documents\Python\cg_reports_root\eod_reports\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.franco\Documents\Python\cg_reports_root\input\eod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B61B65-3962-4025-B65C-14955D6478DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686172B5-E264-4BF6-9D2E-436DB7D82C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="3255" windowWidth="21600" windowHeight="11295" xr2:uid="{B00F3ABA-4ADF-4F8B-953B-44080F46F3AD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B00F3ABA-4ADF-4F8B-953B-44080F46F3AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,14 +93,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,41 +176,44 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="18" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="18" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -811,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746EE0D4-F611-49C2-B013-2E50BF349C53}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15"/>
@@ -826,52 +821,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75">
-      <c r="B1" s="2">
-        <v>45539</v>
-      </c>
-      <c r="C1" s="2">
-        <v>45540</v>
-      </c>
-      <c r="D1" s="2">
-        <v>45541</v>
-      </c>
-      <c r="E1" s="2">
-        <v>45544</v>
-      </c>
-      <c r="F1" s="2">
-        <v>45545</v>
+      <c r="B1" s="11">
+        <v>45576</v>
+      </c>
+      <c r="C1" s="11">
+        <v>45579</v>
+      </c>
+      <c r="D1" s="11">
+        <v>45580</v>
+      </c>
+      <c r="E1" s="11">
+        <v>45581</v>
+      </c>
+      <c r="F1" s="11">
+        <v>45582</v>
       </c>
       <c r="G1" s="3"/>
       <c r="I1" s="2">
-        <v>45539</v>
+        <v>45576</v>
       </c>
       <c r="J1" s="2">
-        <v>45540</v>
-      </c>
-      <c r="K1" s="4">
-        <v>45541</v>
+        <v>45579</v>
+      </c>
+      <c r="K1" s="2">
+        <v>45580</v>
       </c>
       <c r="L1" s="2">
-        <v>45544</v>
+        <v>45581</v>
       </c>
       <c r="M1" s="2">
-        <v>45545</v>
+        <v>45582</v>
       </c>
       <c r="N1" s="3"/>
-      <c r="P1" s="4">
-        <v>45539</v>
-      </c>
-      <c r="Q1" s="4">
-        <v>45540</v>
-      </c>
-      <c r="R1" s="4">
-        <v>45541</v>
+      <c r="P1" s="2">
+        <v>45576</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>45579</v>
+      </c>
+      <c r="R1" s="2">
+        <v>45580</v>
       </c>
       <c r="S1" s="2">
-        <v>45544</v>
+        <v>45581</v>
       </c>
       <c r="T1" s="2">
-        <v>45545</v>
+        <v>45582</v>
       </c>
       <c r="U1" s="3"/>
     </row>
@@ -879,28 +874,28 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="12">
         <v>1500</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="12">
         <v>1500</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="12">
         <v>1500</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="12">
         <v>1500</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="12">
         <v>1500</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="1">
         <v>500</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="1">
         <v>500</v>
       </c>
       <c r="K2" s="1">
@@ -915,19 +910,19 @@
       <c r="O2" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="13">
         <v>1000</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="13">
         <v>1000</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="13">
         <v>1000</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" s="13">
         <v>1000</v>
       </c>
-      <c r="T2" s="1">
+      <c r="T2" s="13">
         <v>1000</v>
       </c>
     </row>
@@ -935,147 +930,147 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
-        <v>2762</v>
-      </c>
-      <c r="C3" s="5">
-        <v>6938</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5625</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4156</v>
-      </c>
-      <c r="F3" s="1">
-        <v>3523</v>
+      <c r="B3" s="12">
+        <v>1509</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2609</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2500</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1537</v>
+      </c>
+      <c r="F3" s="12">
+        <v>1099</v>
       </c>
       <c r="H3" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="5">
-        <v>593</v>
-      </c>
-      <c r="J3" s="5">
-        <v>530</v>
+      <c r="I3" s="1">
+        <v>358</v>
+      </c>
+      <c r="J3" s="1">
+        <v>545</v>
       </c>
       <c r="K3" s="1">
-        <v>281</v>
+        <v>563</v>
       </c>
       <c r="L3" s="1">
-        <v>639</v>
+        <v>251</v>
       </c>
       <c r="M3" s="1">
-        <v>388</v>
+        <v>306</v>
       </c>
       <c r="O3" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="5">
-        <v>459</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>558</v>
+      <c r="P3" s="1">
+        <v>458</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>688</v>
       </c>
       <c r="R3" s="1">
+        <v>485</v>
+      </c>
+      <c r="S3" s="1">
         <v>275</v>
       </c>
-      <c r="S3" s="1">
-        <v>757</v>
-      </c>
       <c r="T3" s="1">
-        <v>440</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>84</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>77</v>
-      </c>
-      <c r="F4" s="1">
-        <v>12</v>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="5">
-        <v>818</v>
-      </c>
-      <c r="J4" s="5">
-        <v>524</v>
+      <c r="I4" s="1">
+        <v>350</v>
+      </c>
+      <c r="J4" s="1">
+        <v>867</v>
       </c>
       <c r="K4" s="1">
-        <v>269</v>
+        <v>563</v>
       </c>
       <c r="L4" s="1">
-        <v>803</v>
+        <v>250</v>
       </c>
       <c r="M4" s="1">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="O4" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="5">
-        <v>396</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>510</v>
+      <c r="P4" s="1">
+        <v>468</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>537</v>
       </c>
       <c r="R4" s="1">
-        <v>250</v>
+        <v>410</v>
       </c>
       <c r="S4" s="1">
-        <v>772</v>
+        <v>119</v>
       </c>
       <c r="T4" s="1">
-        <v>341</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
-        <v>6106</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1932</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>354</v>
+      <c r="B5" s="12">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="5">
-        <v>224</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0</v>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>317</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
       </c>
       <c r="L5" s="1">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
@@ -1083,10 +1078,10 @@
       <c r="O5" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="5">
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
         <v>0</v>
       </c>
       <c r="R5" s="1">
@@ -1103,85 +1098,85 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5">
-        <v>109</v>
-      </c>
-      <c r="C6" s="5">
-        <v>149</v>
-      </c>
-      <c r="D6" s="1">
-        <v>233</v>
-      </c>
-      <c r="E6" s="1">
-        <v>209</v>
-      </c>
-      <c r="F6" s="1">
-        <v>310</v>
+      <c r="B6" s="12">
+        <v>360</v>
+      </c>
+      <c r="C6" s="12">
+        <v>390</v>
+      </c>
+      <c r="D6" s="12">
+        <v>406</v>
+      </c>
+      <c r="E6" s="12">
+        <v>413</v>
+      </c>
+      <c r="F6" s="12">
+        <v>421</v>
       </c>
       <c r="H6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0</v>
+      <c r="I6" s="1">
+        <v>7</v>
+      </c>
+      <c r="J6" s="1">
+        <v>53</v>
       </c>
       <c r="K6" s="1">
+        <v>12</v>
+      </c>
+      <c r="L6" s="1">
         <v>2</v>
       </c>
-      <c r="L6" s="1">
-        <v>4</v>
-      </c>
       <c r="M6" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O6" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="5">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>97</v>
+      <c r="P6" s="1">
+        <v>84</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>57</v>
       </c>
       <c r="R6" s="1">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="S6" s="1">
-        <v>132</v>
+        <v>18</v>
       </c>
       <c r="T6" s="1">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1872</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1321</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1979</v>
-      </c>
-      <c r="F7" s="1">
-        <v>460</v>
+      <c r="B7" s="12">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12">
+        <v>384</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0</v>
       </c>
       <c r="H7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="5">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0</v>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
@@ -1190,226 +1185,226 @@
         <v>0</v>
       </c>
       <c r="M7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" t="s">
         <v>3</v>
       </c>
-      <c r="P7" s="5">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>185</v>
+      <c r="P7" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>50</v>
       </c>
       <c r="R7" s="1">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="S7" s="1">
-        <v>166</v>
+        <v>19</v>
       </c>
       <c r="T7" s="1">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="5">
-        <v>2760</v>
-      </c>
-      <c r="C8" s="5">
-        <v>4833</v>
+      <c r="B8" s="4">
+        <v>2279</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1473</v>
       </c>
       <c r="D8" s="1">
-        <v>4071</v>
+        <v>1525</v>
       </c>
       <c r="E8" s="1">
-        <v>1891</v>
+        <v>1515</v>
       </c>
       <c r="F8" s="1">
-        <v>2741</v>
+        <v>1090</v>
       </c>
       <c r="H8" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <f>(I3/I2)*100</f>
-        <v>118.6</v>
-      </c>
-      <c r="J8" s="6">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="J8" s="5">
         <f>(J3/J2)*100</f>
-        <v>106</v>
-      </c>
-      <c r="K8" s="6">
+        <v>109.00000000000001</v>
+      </c>
+      <c r="K8" s="5">
         <f>(K3/K2)*100</f>
-        <v>56.2</v>
-      </c>
-      <c r="L8" s="6">
+        <v>112.6</v>
+      </c>
+      <c r="L8" s="5">
         <f t="shared" ref="L8:M8" si="0">(L3/L2)*100</f>
-        <v>127.8</v>
-      </c>
-      <c r="M8" s="6">
+        <v>50.2</v>
+      </c>
+      <c r="M8" s="5">
         <f t="shared" si="0"/>
-        <v>77.600000000000009</v>
+        <v>61.199999999999996</v>
       </c>
       <c r="O8" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="5">
         <f>(P3/P2)*100</f>
-        <v>45.9</v>
-      </c>
-      <c r="Q8" s="6">
+        <v>45.800000000000004</v>
+      </c>
+      <c r="Q8" s="5">
         <f>(Q3/Q2)*100</f>
-        <v>55.800000000000004</v>
-      </c>
-      <c r="R8" s="6">
+        <v>68.8</v>
+      </c>
+      <c r="R8" s="5">
         <f>(R3/R2)*100</f>
+        <v>48.5</v>
+      </c>
+      <c r="S8" s="5">
+        <f t="shared" ref="S8:T8" si="1">(S3/S2)*100</f>
         <v>27.500000000000004</v>
       </c>
-      <c r="S8" s="6">
-        <f t="shared" ref="S8:T8" si="1">(S3/S2)*100</f>
-        <v>75.7</v>
-      </c>
-      <c r="T8" s="6">
+      <c r="T8" s="5">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <f>(B8/B2)*100</f>
-        <v>184</v>
-      </c>
-      <c r="C9" s="6">
+        <v>151.93333333333334</v>
+      </c>
+      <c r="C9" s="5">
         <f>(C8/C2)*100</f>
-        <v>322.2</v>
-      </c>
-      <c r="D9" s="6">
+        <v>98.2</v>
+      </c>
+      <c r="D9" s="5">
         <f>(D8/D2)*100</f>
-        <v>271.39999999999998</v>
-      </c>
-      <c r="E9" s="6">
+        <v>101.66666666666666</v>
+      </c>
+      <c r="E9" s="5">
         <f>(E8/E2)*100</f>
-        <v>126.06666666666666</v>
-      </c>
-      <c r="F9" s="6">
+        <v>101</v>
+      </c>
+      <c r="F9" s="5">
         <f>(F8/F2)*100</f>
-        <v>182.73333333333332</v>
+        <v>72.666666666666671</v>
       </c>
       <c r="H9" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <f>I3/(I4-I7)*100</f>
-        <v>72.58261933904528</v>
-      </c>
-      <c r="J9" s="6">
+        <v>102.28571428571429</v>
+      </c>
+      <c r="J9" s="5">
         <f>J3/(J4-J7)*100</f>
-        <v>101.14503816793894</v>
-      </c>
-      <c r="K9" s="6">
+        <v>63.225058004640367</v>
+      </c>
+      <c r="K9" s="5">
         <f>K3/(K4-K7)*100</f>
-        <v>104.46096654275092</v>
-      </c>
-      <c r="L9" s="6">
+        <v>100</v>
+      </c>
+      <c r="L9" s="5">
         <f t="shared" ref="L9:M9" si="2">L3/(L4-L7)*100</f>
-        <v>79.576587795765874</v>
-      </c>
-      <c r="M9" s="6">
+        <v>100.4</v>
+      </c>
+      <c r="M9" s="5">
         <f t="shared" si="2"/>
-        <v>106.5934065934066</v>
+        <v>100.32786885245901</v>
       </c>
       <c r="O9" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="5">
         <f>P3/(P4-P7)*100</f>
-        <v>120.15706806282722</v>
-      </c>
-      <c r="Q9" s="6">
+        <v>104.56621004566212</v>
+      </c>
+      <c r="Q9" s="5">
         <f>Q3/(Q4-Q7)*100</f>
-        <v>171.69230769230771</v>
-      </c>
-      <c r="R9" s="6">
+        <v>141.27310061601642</v>
+      </c>
+      <c r="R9" s="5">
         <f>R3/(R4-R7)*100</f>
-        <v>117.52136752136752</v>
-      </c>
-      <c r="S9" s="6">
+        <v>133.24175824175825</v>
+      </c>
+      <c r="S9" s="5">
         <f t="shared" ref="S9:T9" si="3">S3/(S4-S7)*100</f>
-        <v>124.91749174917493</v>
-      </c>
-      <c r="T9" s="6">
+        <v>275</v>
+      </c>
+      <c r="T9" s="5">
         <f t="shared" si="3"/>
-        <v>135.38461538461539</v>
+        <v>110.00000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <f>B8/(B3-B6-B4)*100</f>
-        <v>104.0331699962307</v>
-      </c>
-      <c r="C10" s="6">
+        <v>198.34638816362053</v>
+      </c>
+      <c r="C10" s="5">
         <f>C8/(C3-C6-C4)*100</f>
-        <v>72.080536912751683</v>
-      </c>
-      <c r="D10" s="6">
+        <v>66.381252816584052</v>
+      </c>
+      <c r="D10" s="5">
         <f>D8/(D3-D6-D4)*100</f>
-        <v>75.500741839762611</v>
-      </c>
-      <c r="E10" s="6">
+        <v>72.827125119388725</v>
+      </c>
+      <c r="E10" s="5">
         <f>E8/(E3-E6-E4)*100</f>
-        <v>48.863049095607238</v>
-      </c>
-      <c r="F10" s="6">
+        <v>134.90650044523596</v>
+      </c>
+      <c r="F10" s="5">
         <f>F8/(F3-F6-F4)*100</f>
-        <v>85.629490784129956</v>
+        <v>160.7669616519174</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75">
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Q13" s="7" t="s">
+      <c r="Q13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>0.95000000000000007</v>
       </c>
-      <c r="D15" s="10" t="b">
+      <c r="D15" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K15" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" s="8" t="s">
+      <c r="K15" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P15" s="9">
+      <c r="P15" s="8">
         <v>0.95000000000000007</v>
       </c>
-      <c r="R15" s="10" t="b">
+      <c r="R15" s="9" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>